<commit_message>
Hill formulas are updates
</commit_message>
<xml_diff>
--- a/Data/Perovskite dataset.xlsx
+++ b/Data/Perovskite dataset.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -2798,42 +2798,6 @@
     <t>Ba2 H Nb3 O10</t>
   </si>
   <si>
-    <t>H3 Nb3 O20 Sr2</t>
-  </si>
-  <si>
-    <t>H5 Me N Nb3 O20 Sr2</t>
-  </si>
-  <si>
-    <t>Et H5 N Nb3 O20 Sr2</t>
-  </si>
-  <si>
-    <t>H5 N Nb3 O20 Pr Sr2</t>
-  </si>
-  <si>
-    <t>Bu H5 N Nb3 O20 Sr2</t>
-  </si>
-  <si>
-    <t>H5 Hx N Nb3 O20 Sr2</t>
-  </si>
-  <si>
-    <t>H5 N Nb3 O20 Oc Sr2</t>
-  </si>
-  <si>
-    <t>H4 Me Nb3 O21 Sr2</t>
-  </si>
-  <si>
-    <t>Et H4 Nb3 O21 Sr2</t>
-  </si>
-  <si>
-    <t>H4 Nb3 O21 Pr Sr2</t>
-  </si>
-  <si>
-    <t>Bu H4 Nb3 O21 Sr2</t>
-  </si>
-  <si>
-    <t>H4 Hx Nb3 O21 Sr2</t>
-  </si>
-  <si>
     <t>La2 Li2 O10 Ti3</t>
   </si>
   <si>
@@ -2849,12 +2813,6 @@
     <t>K2 Nd2 O10 Ti3</t>
   </si>
   <si>
-    <t>Ca2 K Nan Nb3 O10</t>
-  </si>
-  <si>
-    <t>Ca2 K Na Nb4 O12</t>
-  </si>
-  <si>
     <t>Ca2 Nb2 O10 Ta</t>
   </si>
   <si>
@@ -2876,99 +2834,9 @@
     <t>H La O4 Ti</t>
   </si>
   <si>
-    <t>H3 La Me N O4 Ti</t>
-  </si>
-  <si>
-    <t>Et H3 La N O4 Ti</t>
-  </si>
-  <si>
-    <t>H3 La N O4 Pr Ti</t>
-  </si>
-  <si>
-    <t>Bu H3 La N O4 Ti</t>
-  </si>
-  <si>
-    <t>H3 Hx La N O4 Ti</t>
-  </si>
-  <si>
-    <t>H3 La N O4 Ox Ti</t>
-  </si>
-  <si>
-    <t>H2 La Me O5 Ti</t>
-  </si>
-  <si>
-    <t>Et H2 La O5 Ti</t>
-  </si>
-  <si>
-    <t>H2 La O5 Pr Ti</t>
-  </si>
-  <si>
-    <t>Bu H2 La O5 Ti</t>
-  </si>
-  <si>
-    <t>H2 Hx La O5 Ti</t>
-  </si>
-  <si>
-    <t>H2 La O5 Ox Ti</t>
-  </si>
-  <si>
     <t>H Nd O4 Ti</t>
   </si>
   <si>
-    <t>H3 Me N Nd O4 Ti</t>
-  </si>
-  <si>
-    <t>Et H3 N Nd O4 Ti</t>
-  </si>
-  <si>
-    <t>H3 N Nd O4 Pr Ti</t>
-  </si>
-  <si>
-    <t>Bu H3 N Nd O4 Ti</t>
-  </si>
-  <si>
-    <t>H3 Hx N Nd O4 Ti</t>
-  </si>
-  <si>
-    <t>H3 N Nd O4 Ox Ti</t>
-  </si>
-  <si>
-    <t>H2 Me Nd O5 Ti</t>
-  </si>
-  <si>
-    <t>Et H2 Nd O5 Ti</t>
-  </si>
-  <si>
-    <t>H2 Nd O5 Pr Ti</t>
-  </si>
-  <si>
-    <t>Bu H2 Nd O5 Ti</t>
-  </si>
-  <si>
-    <t>H2 Hx Nd O5 Ti</t>
-  </si>
-  <si>
-    <t>H2 Nd O5 Ox Ti</t>
-  </si>
-  <si>
-    <t>Ca2 H2 Me Nb3 O11</t>
-  </si>
-  <si>
-    <t>Ca2 Et H2 Nb3 O11</t>
-  </si>
-  <si>
-    <t>Ca2 H2 Nb3 O11 Pr</t>
-  </si>
-  <si>
-    <t>Bu Ca2 H2 Nb3 O11</t>
-  </si>
-  <si>
-    <t>Ca2 H2 Hx Nb3 O11</t>
-  </si>
-  <si>
-    <t>Ca2 H2 Nb3 O11 Ox</t>
-  </si>
-  <si>
     <t>H2 La2 O10 Ti3</t>
   </si>
   <si>
@@ -2978,135 +2846,12 @@
     <t>K Nd O7 Ta2</t>
   </si>
   <si>
-    <t>Bu Ca2 H3 N Nb3 O11</t>
-  </si>
-  <si>
-    <t>Ca2 Et H2 Nb3 O13</t>
-  </si>
-  <si>
     <t>H La2 O10 Ti3</t>
   </si>
   <si>
-    <t>Et H3 La2 N O10 Ti3</t>
-  </si>
-  <si>
-    <t>Et H2 La2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>Ca2 H3 Me N Nb3 O10</t>
-  </si>
-  <si>
-    <t>Ca2 Et H3 N Nb3 O10</t>
-  </si>
-  <si>
-    <t>Ca2 H3 N Nb3 O10 Pr</t>
-  </si>
-  <si>
-    <t>Bu Ca2 H3 N Nb3 O10</t>
-  </si>
-  <si>
-    <t>Ca2 H3 Hx N Nb3 O10</t>
-  </si>
-  <si>
-    <t>Ca2 H3 N Nb3 O10 Oc</t>
-  </si>
-  <si>
-    <t>H4 La2 Me N O10 Ti3</t>
-  </si>
-  <si>
-    <t>Et H4 La2 N O10 Ti3</t>
-  </si>
-  <si>
-    <t>H4 La2 N O10 Pr Ti3</t>
-  </si>
-  <si>
-    <t>Bu H4 La2 N O10 Ti3</t>
-  </si>
-  <si>
-    <t>H4 Hx La2 N O10 Ti3</t>
-  </si>
-  <si>
-    <t>H4 La2 N O10 Oc Ti3</t>
-  </si>
-  <si>
-    <t>H3 La2 Me O11 Ti3</t>
-  </si>
-  <si>
-    <t>Et H3 La2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>H3 La2 O11 Pr Ti3</t>
-  </si>
-  <si>
-    <t>Bu H3 La2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>H3 Hx La2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>H3 La2 O11 Oc Ti3</t>
-  </si>
-  <si>
     <t>H2 Nd2 O10 Ti3</t>
   </si>
   <si>
-    <t>H4 Me N Nd2 O10 Ti3</t>
-  </si>
-  <si>
-    <t>Et H4 N Nd2 O10 Ti3</t>
-  </si>
-  <si>
-    <t>H4 N Nd2 O10 Pr Ti3</t>
-  </si>
-  <si>
-    <t>Bu H4 N Nd2 O10 Ti3</t>
-  </si>
-  <si>
-    <t>H4 Hx N Nd2 O10 Ti3</t>
-  </si>
-  <si>
-    <t>H4 N Nd2 O10 Oc Ti3</t>
-  </si>
-  <si>
-    <t>H3 Me Nd2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>Et H3 Nd2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>H3 Nd2 O11 Pr Ti3</t>
-  </si>
-  <si>
-    <t>Bu H3 Nd2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>H3 Hx Nd2 O11 Ti3</t>
-  </si>
-  <si>
-    <t>H3 Nd2 O11 Oc Ti3</t>
-  </si>
-  <si>
-    <t>Bi2 H4 K O14 Ti4</t>
-  </si>
-  <si>
-    <t>Bi2 H6 K Me N O14 Ti4</t>
-  </si>
-  <si>
-    <t>Bi2 Et H7 K N O14 Ti4</t>
-  </si>
-  <si>
-    <t>Bi2 H8 K N O14 Pr Ti4</t>
-  </si>
-  <si>
-    <t>Bi2 Bu H9 K N O14 Ti4</t>
-  </si>
-  <si>
-    <t>Bi2 H10 Hx K N O14 Ti4</t>
-  </si>
-  <si>
-    <t>Bi2 H11 K N O14 Oc Ti4</t>
-  </si>
-  <si>
     <t>Ca O3 Ti</t>
   </si>
   <si>
@@ -3152,15 +2897,6 @@
     <t>Bi4 Cl Nb O11 Pb Ti</t>
   </si>
   <si>
-    <t>Ca2 H3 Me N Nb3 O10 Pt</t>
-  </si>
-  <si>
-    <t>Bu Ca2 H3 N Nb3 O10 Pt</t>
-  </si>
-  <si>
-    <t>Ca2 H3 N Nb3 O10 Oc Pt</t>
-  </si>
-  <si>
     <t>1 C6H13NH2</t>
   </si>
   <si>
@@ -3269,9 +3005,6 @@
     <t>Ca1.5 K0.5 La0.5 Nb3 O10</t>
   </si>
   <si>
-    <t>Ca0.75 K0.5 La0.5 Nb3 O10</t>
-  </si>
-  <si>
     <t>Bi0.25 Ca0.75 K0.5 La0.25 Nb3 O10 Pb0.75</t>
   </si>
   <si>
@@ -3485,18 +3218,6 @@
     <t>N, Nb4+</t>
   </si>
   <si>
-    <t>KCa2Na2Nb5O15</t>
-  </si>
-  <si>
-    <t>KCa2Na3Nb6O18</t>
-  </si>
-  <si>
-    <t>Ca2 K Na2 Nb5 O15</t>
-  </si>
-  <si>
-    <t>Ca2 K Na3 Nb6 O18</t>
-  </si>
-  <si>
     <t>Ca1.5 H Nb3 O10 Sr0.5</t>
   </si>
   <si>
@@ -3582,19 +3303,305 @@
   </si>
   <si>
     <t>Без ID</t>
+  </si>
+  <si>
+    <t>K0.5La0.5Ca0.75Pn0.75Nb3O10</t>
+  </si>
+  <si>
+    <t>Ca0.75 K0.5 La0.5 Nb3 O10 Pb0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C H5 N Nb3 O20 Sr2 </t>
+  </si>
+  <si>
+    <t>H Nb3 O19 Sr2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C H6 N Nb3 O19 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8 H20 N Nb3 O19 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6 H16 N Nb3 O19 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4 H12 N Nb3 O19 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3 H10 N Nb3 O19 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2 H8 N Nb3 O19 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2 H7 N Nb3 O20 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3 H9 N Nb3 O20 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4 H11 N Nb3 O20 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6 H15 N Nb3 O20 Sr2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8 H19 N Nb3 O20 Sr2 </t>
+  </si>
+  <si>
+    <t>Ca2 K Na2 Nb5 O16</t>
+  </si>
+  <si>
+    <t>Ca2 K Na3 Nb6 O19</t>
+  </si>
+  <si>
+    <t>KNaCa2Nb4O13</t>
+  </si>
+  <si>
+    <t>KNa2Ca2Nb5O16</t>
+  </si>
+  <si>
+    <t>KNa3Ca2Nb6O19</t>
+  </si>
+  <si>
+    <t>H6 C La N O4 Ti</t>
+  </si>
+  <si>
+    <t>H8 C2 La N O4 Ti</t>
+  </si>
+  <si>
+    <t>H10 C3 La N O4 Ti</t>
+  </si>
+  <si>
+    <t>H12 C4 La N O4 Ti</t>
+  </si>
+  <si>
+    <t>H20 C8 La N O4 Ti</t>
+  </si>
+  <si>
+    <t>H16 C6 La N O4 Ti</t>
+  </si>
+  <si>
+    <t>H19 C8 La O5 Ti</t>
+  </si>
+  <si>
+    <t>H15 C6 La O5 Ti</t>
+  </si>
+  <si>
+    <t>H11 C4 La O5 Ti</t>
+  </si>
+  <si>
+    <t>H9 C3 La O5 Ti</t>
+  </si>
+  <si>
+    <t>H7 C2 La O5 Ti</t>
+  </si>
+  <si>
+    <t>H5 C La O5 Ti</t>
+  </si>
+  <si>
+    <t>H6 C Nd N O4 Ti</t>
+  </si>
+  <si>
+    <t>H8 C2 Nd N O4 Ti</t>
+  </si>
+  <si>
+    <t>H10 C3 Nd N O4 Ti</t>
+  </si>
+  <si>
+    <t>H12 C4 Nd N O4 Ti</t>
+  </si>
+  <si>
+    <t>H16 C6 Nd N O4 Ti</t>
+  </si>
+  <si>
+    <t>H20 C8 Nd N O4 Ti</t>
+  </si>
+  <si>
+    <t>H5 C Nd O5 Ti</t>
+  </si>
+  <si>
+    <t>H7 C2 Nd O5 Ti</t>
+  </si>
+  <si>
+    <t>H9 C3 Nd O5 Ti</t>
+  </si>
+  <si>
+    <t>H11 C4 Nd O5 Ti</t>
+  </si>
+  <si>
+    <t>H15 C6 Nd O5 Ti</t>
+  </si>
+  <si>
+    <t>H19 C8 Nd O5 Ti</t>
+  </si>
+  <si>
+    <t>C Ca2 H5 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C2 Ca2 H7 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C3 Ca2 H9 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C4 Ca2 H11 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C6 Ca2 H15 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C8 Ca2 H19 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C4 H12 Ca2 N Nb3 O10</t>
+  </si>
+  <si>
+    <t>C2 H7 Ca2 Nb3 O11</t>
+  </si>
+  <si>
+    <t>C2 H8 La2 N O10 Ti3</t>
+  </si>
+  <si>
+    <t>C2 H7 La2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C Ca2 H6 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C2 Ca2 H8 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C3 Ca2 H10 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C4 Ca2 H12 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C6 Ca2 H16 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C8 Ca2 H20 Nb3 O10</t>
+  </si>
+  <si>
+    <t>C H6 La2 N O10 Ti3</t>
+  </si>
+  <si>
+    <t>C3 H10 La2 N O10 Ti3</t>
+  </si>
+  <si>
+    <t>C4 H12 La2 N O10 Ti3</t>
+  </si>
+  <si>
+    <t>C6 H16 La2 N O10 Ti3</t>
+  </si>
+  <si>
+    <t>C8 H20 La2 N O10 Ti3</t>
+  </si>
+  <si>
+    <t>C H5 La2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C3 H9 La2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C4 H11 La2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C6 H15 La2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C8 H19 La2 O11Ti3</t>
+  </si>
+  <si>
+    <t>C H7 Nd2 O10 Ti3</t>
+  </si>
+  <si>
+    <t>C2 H9 Nd2 O10 Ti3</t>
+  </si>
+  <si>
+    <t>C3 H11 Nd2 O10 Ti3</t>
+  </si>
+  <si>
+    <t>C4 H13 Nd2 O10 Ti3</t>
+  </si>
+  <si>
+    <t>C6 H17 Nd2 O10 Ti3</t>
+  </si>
+  <si>
+    <t>C8 H21 Nd2 O10 Ti3</t>
+  </si>
+  <si>
+    <t>C H6 Nd2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C2 H8 Nd2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C3 H10 Nd2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C4 H12 Nd2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C6 H16 Nd2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>C8 H20 Nd2 O11 Ti3</t>
+  </si>
+  <si>
+    <t>Bi2 H4 K O13 Ti4</t>
+  </si>
+  <si>
+    <t>C Bi2 H7 K0.5 O13 Ti4</t>
+  </si>
+  <si>
+    <t>C2 Bi2.5 H9 K0.5 O13 Ti4</t>
+  </si>
+  <si>
+    <t>C3 Bi2.5 H11 K0.5 O13 Ti4</t>
+  </si>
+  <si>
+    <t>C4 Bi2.5 H13 K0.5 O13 Ti4</t>
+  </si>
+  <si>
+    <t>C6 Bi2.5 H17 K0.5 O13 Ti4</t>
+  </si>
+  <si>
+    <t>C8 Bi2.5 H21 K0.5 O13 Ti4</t>
+  </si>
+  <si>
+    <t>C4 H13 N Nd2 O10 Ti3</t>
+  </si>
+  <si>
+    <t>C Ca2 H6 N Nb3 O10</t>
+  </si>
+  <si>
+    <t>C4 Ca2 H12 N Nb3 O10</t>
+  </si>
+  <si>
+    <t>C8 Ca2 H20 N Nb3 O10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3721,42 +3728,43 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -3805,7 +3813,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4850,7 +4857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4860,16 +4867,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH527"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="A2:AH527"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A404" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C531" sqref="C531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.21875" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
@@ -4898,13 +4905,13 @@
         <v>784</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>1099</v>
+        <v>1010</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>775</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1081</v>
+        <v>993</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>130</v>
@@ -6308,7 +6315,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>1077</v>
+        <v>989</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="2"/>
@@ -6367,7 +6374,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>1078</v>
+        <v>990</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="2"/>
@@ -6424,7 +6431,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>1079</v>
+        <v>991</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="2"/>
@@ -6546,7 +6553,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>1080</v>
+        <v>992</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="2"/>
@@ -7158,7 +7165,7 @@
         <v>33</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>1082</v>
+        <v>994</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="2"/>
@@ -7218,10 +7225,10 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>1083</v>
+        <v>1095</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>1096</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="2"/>
@@ -7282,7 +7289,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>1084</v>
+        <v>995</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="2"/>
@@ -8673,7 +8680,7 @@
         <v>777</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>1100</v>
+        <v>1011</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="2"/>
@@ -9289,7 +9296,7 @@
         <v>66</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>1101</v>
+        <v>1012</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="2"/>
@@ -9360,10 +9367,10 @@
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>1085</v>
+        <v>996</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>1102</v>
+        <v>1013</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="2"/>
@@ -9434,10 +9441,10 @@
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>1086</v>
+        <v>997</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>1103</v>
+        <v>1014</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="2"/>
@@ -9508,10 +9515,10 @@
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>1087</v>
+        <v>998</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>1104</v>
+        <v>1015</v>
       </c>
       <c r="C81" s="15"/>
       <c r="D81" s="2"/>
@@ -9582,10 +9589,10 @@
     </row>
     <row r="82" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>1088</v>
+        <v>999</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>1105</v>
+        <v>1016</v>
       </c>
       <c r="C82" s="15"/>
       <c r="D82" s="2"/>
@@ -9719,7 +9726,7 @@
         <v>779</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>1106</v>
+        <v>1017</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>781</v>
@@ -9775,7 +9782,7 @@
         <v>780</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>1107</v>
+        <v>1018</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>782</v>
@@ -9826,13 +9833,13 @@
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>1048</v>
+        <v>960</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>1108</v>
+        <v>1019</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>1047</v>
+        <v>959</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -10184,7 +10191,7 @@
         <v>82</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>1109</v>
+        <v>1020</v>
       </c>
       <c r="C92" s="15"/>
       <c r="D92" s="2"/>
@@ -10237,7 +10244,7 @@
         <v>86</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>1110</v>
+        <v>1021</v>
       </c>
       <c r="C93" s="15"/>
       <c r="D93" s="2"/>
@@ -10290,7 +10297,7 @@
         <v>85</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>1111</v>
+        <v>1022</v>
       </c>
       <c r="C94" s="15"/>
       <c r="D94" s="2"/>
@@ -10343,7 +10350,7 @@
         <v>84</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>1112</v>
+        <v>1023</v>
       </c>
       <c r="C95" s="15"/>
       <c r="D95" s="2"/>
@@ -10643,7 +10650,7 @@
         <v>90</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>1113</v>
+        <v>1024</v>
       </c>
       <c r="C100" s="15"/>
       <c r="D100" s="2"/>
@@ -10700,7 +10707,7 @@
         <v>92</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>1114</v>
+        <v>1025</v>
       </c>
       <c r="C101" s="15"/>
       <c r="D101" s="2"/>
@@ -10758,7 +10765,7 @@
         <v>93</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>1115</v>
+        <v>1026</v>
       </c>
       <c r="C102" s="15"/>
       <c r="D102" s="2"/>
@@ -10816,7 +10823,7 @@
         <v>94</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>1116</v>
+        <v>1027</v>
       </c>
       <c r="C103" s="15"/>
       <c r="D103" s="2"/>
@@ -10874,7 +10881,7 @@
         <v>95</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>1117</v>
+        <v>1028</v>
       </c>
       <c r="C104" s="15"/>
       <c r="D104" s="2"/>
@@ -10932,7 +10939,7 @@
         <v>96</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>1118</v>
+        <v>1029</v>
       </c>
       <c r="C105" s="15"/>
       <c r="D105" s="2"/>
@@ -10990,7 +10997,7 @@
         <v>97</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>1119</v>
+        <v>1030</v>
       </c>
       <c r="C106" s="15"/>
       <c r="D106" s="2"/>
@@ -11172,10 +11179,10 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>1049</v>
+        <v>961</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>1120</v>
+        <v>1031</v>
       </c>
       <c r="C109" s="15"/>
       <c r="D109" s="2"/>
@@ -11235,10 +11242,10 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>1050</v>
+        <v>962</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>1121</v>
+        <v>1032</v>
       </c>
       <c r="C110" s="15"/>
       <c r="D110" s="2"/>
@@ -11348,10 +11355,10 @@
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>1057</v>
+        <v>969</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>1054</v>
+        <v>966</v>
       </c>
       <c r="C112" s="15"/>
       <c r="D112" s="2"/>
@@ -11411,10 +11418,10 @@
     </row>
     <row r="113" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>1058</v>
+        <v>970</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>1055</v>
+        <v>967</v>
       </c>
       <c r="C113" s="15"/>
       <c r="D113" s="2"/>
@@ -11472,10 +11479,10 @@
     </row>
     <row r="114" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>1051</v>
+        <v>963</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>1052</v>
+        <v>964</v>
       </c>
       <c r="C114" s="15"/>
       <c r="D114" s="2"/>
@@ -11487,7 +11494,7 @@
         <v>107</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>1053</v>
+        <v>965</v>
       </c>
       <c r="I114">
         <v>1540895</v>
@@ -11581,7 +11588,7 @@
         <v>108</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>1122</v>
+        <v>1033</v>
       </c>
       <c r="C116" s="15"/>
       <c r="D116" s="2"/>
@@ -11923,10 +11930,10 @@
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>1123</v>
+        <v>1034</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>1125</v>
+        <v>1036</v>
       </c>
       <c r="C122" s="15"/>
       <c r="D122" s="2"/>
@@ -11983,10 +11990,10 @@
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>1124</v>
+        <v>1035</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>1126</v>
+        <v>1037</v>
       </c>
       <c r="C123" s="15"/>
       <c r="D123" s="2"/>
@@ -12033,14 +12040,14 @@
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>1124</v>
+        <v>1035</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>1126</v>
+        <v>1037</v>
       </c>
       <c r="C124" s="15"/>
       <c r="D124" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124" s="2">
@@ -12973,7 +12980,7 @@
         <v>135</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>1127</v>
+        <v>1038</v>
       </c>
       <c r="C142" s="15"/>
       <c r="D142" s="2"/>
@@ -13035,7 +13042,7 @@
         <v>136</v>
       </c>
       <c r="B143" s="19" t="s">
-        <v>1128</v>
+        <v>1039</v>
       </c>
       <c r="C143" s="15"/>
       <c r="D143" s="2"/>
@@ -13097,7 +13104,7 @@
         <v>137</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>1129</v>
+        <v>1040</v>
       </c>
       <c r="C144" s="15"/>
       <c r="D144" s="2"/>
@@ -13155,7 +13162,7 @@
         <v>138</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>1130</v>
+        <v>1041</v>
       </c>
       <c r="C145" s="15"/>
       <c r="D145" s="2"/>
@@ -13265,7 +13272,7 @@
         <v>141</v>
       </c>
       <c r="B147" s="19" t="s">
-        <v>1131</v>
+        <v>1042</v>
       </c>
       <c r="C147" s="15"/>
       <c r="D147" s="5"/>
@@ -13309,7 +13316,7 @@
         <v>142</v>
       </c>
       <c r="B148" s="19" t="s">
-        <v>1132</v>
+        <v>1043</v>
       </c>
       <c r="C148" s="15"/>
       <c r="D148" s="5"/>
@@ -13353,7 +13360,7 @@
         <v>143</v>
       </c>
       <c r="B149" s="19" t="s">
-        <v>1133</v>
+        <v>1044</v>
       </c>
       <c r="C149" s="15"/>
       <c r="D149" s="5"/>
@@ -13397,7 +13404,7 @@
         <v>137</v>
       </c>
       <c r="B150" s="19" t="s">
-        <v>1134</v>
+        <v>1045</v>
       </c>
       <c r="C150" s="15"/>
       <c r="D150" s="5"/>
@@ -15410,7 +15417,7 @@
       </c>
       <c r="C188" s="15"/>
       <c r="D188" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E188" s="2">
         <v>4</v>
@@ -15466,7 +15473,7 @@
       </c>
       <c r="C189" s="15"/>
       <c r="D189" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E189" s="2">
         <v>4</v>
@@ -15522,7 +15529,7 @@
       </c>
       <c r="C190" s="15"/>
       <c r="D190" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E190" s="2">
         <v>4</v>
@@ -15578,7 +15585,7 @@
       </c>
       <c r="C191" s="15"/>
       <c r="D191" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E191" s="2">
         <v>4</v>
@@ -15634,7 +15641,7 @@
       </c>
       <c r="C192" s="15"/>
       <c r="D192" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E192" s="2">
         <v>4</v>
@@ -16785,7 +16792,7 @@
       </c>
       <c r="C212" s="15"/>
       <c r="D212" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E212" s="2">
         <v>1</v>
@@ -16837,7 +16844,7 @@
       </c>
       <c r="C213" s="15"/>
       <c r="D213" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E213" s="2">
         <v>1</v>
@@ -16889,7 +16896,7 @@
       </c>
       <c r="C214" s="15"/>
       <c r="D214" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E214" s="2">
         <v>1</v>
@@ -16941,7 +16948,7 @@
       </c>
       <c r="C215" s="15"/>
       <c r="D215" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E215" s="2">
         <v>1</v>
@@ -17449,7 +17456,7 @@
         <v>209</v>
       </c>
       <c r="B225" s="19" t="s">
-        <v>1135</v>
+        <v>1046</v>
       </c>
       <c r="C225" s="15"/>
       <c r="D225" s="2"/>
@@ -17500,10 +17507,10 @@
     </row>
     <row r="226" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
-        <v>1059</v>
+        <v>971</v>
       </c>
       <c r="B226" s="19" t="s">
-        <v>1136</v>
+        <v>1047</v>
       </c>
       <c r="C226" s="15"/>
       <c r="D226" s="2"/>
@@ -17557,7 +17564,7 @@
         <v>211</v>
       </c>
       <c r="B227" s="19" t="s">
-        <v>1137</v>
+        <v>1048</v>
       </c>
       <c r="C227" s="15"/>
       <c r="D227" s="2"/>
@@ -17611,7 +17618,7 @@
         <v>212</v>
       </c>
       <c r="B228" s="19" t="s">
-        <v>1138</v>
+        <v>1049</v>
       </c>
       <c r="C228" s="15"/>
       <c r="D228" s="2"/>
@@ -17665,7 +17672,7 @@
         <v>213</v>
       </c>
       <c r="B229" s="19" t="s">
-        <v>1139</v>
+        <v>1050</v>
       </c>
       <c r="C229" s="15"/>
       <c r="D229" s="2"/>
@@ -17719,7 +17726,7 @@
         <v>214</v>
       </c>
       <c r="B230" s="19" t="s">
-        <v>1140</v>
+        <v>1051</v>
       </c>
       <c r="C230" s="15"/>
       <c r="D230" s="2"/>
@@ -17773,7 +17780,7 @@
         <v>215</v>
       </c>
       <c r="B231" s="19" t="s">
-        <v>1141</v>
+        <v>1052</v>
       </c>
       <c r="C231" s="15"/>
       <c r="D231" s="2"/>
@@ -18151,7 +18158,7 @@
         <v>223</v>
       </c>
       <c r="B239" s="15" t="s">
-        <v>1060</v>
+        <v>972</v>
       </c>
       <c r="C239" s="15"/>
       <c r="D239" s="2"/>
@@ -18195,7 +18202,7 @@
         <v>224</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>1061</v>
+        <v>973</v>
       </c>
       <c r="C240" s="15"/>
       <c r="D240" s="2"/>
@@ -18283,7 +18290,7 @@
         <v>225</v>
       </c>
       <c r="B242" s="15" t="s">
-        <v>1062</v>
+        <v>974</v>
       </c>
       <c r="C242" s="15"/>
       <c r="D242" s="2"/>
@@ -18371,7 +18378,7 @@
         <v>226</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>1063</v>
+        <v>975</v>
       </c>
       <c r="C244" s="15"/>
       <c r="D244" s="2"/>
@@ -18547,7 +18554,7 @@
         <v>229</v>
       </c>
       <c r="B248" s="15" t="s">
-        <v>1064</v>
+        <v>976</v>
       </c>
       <c r="C248" s="15"/>
       <c r="D248" s="2"/>
@@ -18591,7 +18598,7 @@
         <v>230</v>
       </c>
       <c r="B249" s="15" t="s">
-        <v>1065</v>
+        <v>977</v>
       </c>
       <c r="C249" s="15"/>
       <c r="D249" s="2"/>
@@ -18683,7 +18690,7 @@
       </c>
       <c r="C251" s="15"/>
       <c r="D251" s="2" t="s">
-        <v>1066</v>
+        <v>978</v>
       </c>
       <c r="E251" s="2"/>
       <c r="F251" s="2">
@@ -18729,7 +18736,7 @@
       </c>
       <c r="C252" s="15"/>
       <c r="D252" s="2" t="s">
-        <v>1067</v>
+        <v>979</v>
       </c>
       <c r="E252" s="2"/>
       <c r="F252" s="2">
@@ -18775,7 +18782,7 @@
       </c>
       <c r="C253" s="15"/>
       <c r="D253" s="2" t="s">
-        <v>1068</v>
+        <v>980</v>
       </c>
       <c r="E253" s="2"/>
       <c r="F253" s="2">
@@ -18821,7 +18828,7 @@
       </c>
       <c r="C254" s="15"/>
       <c r="D254" s="2" t="s">
-        <v>1069</v>
+        <v>981</v>
       </c>
       <c r="E254" s="2"/>
       <c r="F254" s="2">
@@ -18867,7 +18874,7 @@
       </c>
       <c r="C255" s="15"/>
       <c r="D255" s="2" t="s">
-        <v>1070</v>
+        <v>982</v>
       </c>
       <c r="E255" s="2"/>
       <c r="F255" s="2">
@@ -18997,7 +19004,7 @@
         <v>239</v>
       </c>
       <c r="B258" s="19" t="s">
-        <v>1142</v>
+        <v>1053</v>
       </c>
       <c r="C258" s="15"/>
       <c r="D258" s="2"/>
@@ -19041,7 +19048,7 @@
         <v>240</v>
       </c>
       <c r="B259" s="19" t="s">
-        <v>1143</v>
+        <v>1054</v>
       </c>
       <c r="C259" s="15"/>
       <c r="D259" s="2"/>
@@ -19085,7 +19092,7 @@
         <v>241</v>
       </c>
       <c r="B260" s="19" t="s">
-        <v>1144</v>
+        <v>1055</v>
       </c>
       <c r="C260" s="15"/>
       <c r="D260" s="2"/>
@@ -19133,7 +19140,7 @@
       </c>
       <c r="C261" s="15"/>
       <c r="D261" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E261" s="2">
         <v>4</v>
@@ -19177,11 +19184,11 @@
         <v>239</v>
       </c>
       <c r="B262" s="19" t="s">
-        <v>1142</v>
+        <v>1053</v>
       </c>
       <c r="C262" s="15"/>
       <c r="D262" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E262" s="2">
         <v>4</v>
@@ -19225,11 +19232,11 @@
         <v>240</v>
       </c>
       <c r="B263" s="19" t="s">
-        <v>1143</v>
+        <v>1054</v>
       </c>
       <c r="C263" s="15"/>
       <c r="D263" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E263" s="2">
         <v>4</v>
@@ -19273,11 +19280,11 @@
         <v>241</v>
       </c>
       <c r="B264" s="19" t="s">
-        <v>1144</v>
+        <v>1055</v>
       </c>
       <c r="C264" s="15"/>
       <c r="D264" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E264" s="2">
         <v>4</v>
@@ -19321,7 +19328,7 @@
         <v>22</v>
       </c>
       <c r="B265" s="19" t="s">
-        <v>1077</v>
+        <v>989</v>
       </c>
       <c r="C265" s="15"/>
       <c r="D265" s="2"/>
@@ -19365,7 +19372,7 @@
         <v>23</v>
       </c>
       <c r="B266" s="19" t="s">
-        <v>1078</v>
+        <v>990</v>
       </c>
       <c r="C266" s="15"/>
       <c r="D266" s="2"/>
@@ -19409,7 +19416,7 @@
         <v>24</v>
       </c>
       <c r="B267" s="19" t="s">
-        <v>1079</v>
+        <v>991</v>
       </c>
       <c r="C267" s="15"/>
       <c r="D267" s="2"/>
@@ -19497,7 +19504,7 @@
         <v>26</v>
       </c>
       <c r="B269" s="19" t="s">
-        <v>1080</v>
+        <v>992</v>
       </c>
       <c r="C269" s="15"/>
       <c r="D269" s="2"/>
@@ -19633,7 +19640,7 @@
       </c>
       <c r="C272" s="15"/>
       <c r="D272" s="2" t="s">
-        <v>1071</v>
+        <v>983</v>
       </c>
       <c r="E272" s="2"/>
       <c r="F272" s="2">
@@ -19716,10 +19723,10 @@
     </row>
     <row r="274" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
-        <v>1072</v>
+        <v>984</v>
       </c>
       <c r="B274" s="15" t="s">
-        <v>1073</v>
+        <v>985</v>
       </c>
       <c r="C274" s="15"/>
       <c r="D274" s="2"/>
@@ -19903,7 +19910,7 @@
       </c>
       <c r="C278" s="15"/>
       <c r="D278" s="2" t="s">
-        <v>1074</v>
+        <v>986</v>
       </c>
       <c r="E278" s="2"/>
       <c r="F278" s="2">
@@ -20125,7 +20132,7 @@
         <v>264</v>
       </c>
       <c r="B283" s="19" t="s">
-        <v>1145</v>
+        <v>1056</v>
       </c>
       <c r="C283" s="15"/>
       <c r="D283" s="2"/>
@@ -20169,7 +20176,7 @@
         <v>265</v>
       </c>
       <c r="B284" s="19" t="s">
-        <v>1146</v>
+        <v>1057</v>
       </c>
       <c r="C284" s="15"/>
       <c r="D284" s="2"/>
@@ -20305,7 +20312,7 @@
       </c>
       <c r="C287" s="15"/>
       <c r="D287" s="2" t="s">
-        <v>1075</v>
+        <v>987</v>
       </c>
       <c r="E287" s="2"/>
       <c r="F287" s="2">
@@ -20395,7 +20402,7 @@
       </c>
       <c r="C289" s="15"/>
       <c r="D289" s="2" t="s">
-        <v>1076</v>
+        <v>988</v>
       </c>
       <c r="E289" s="2"/>
       <c r="F289" s="2">
@@ -20529,7 +20536,7 @@
       </c>
       <c r="C292" s="15"/>
       <c r="D292" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E292" s="2">
         <v>3</v>
@@ -20711,7 +20718,7 @@
       </c>
       <c r="C296" s="15"/>
       <c r="D296" s="2" t="s">
-        <v>1089</v>
+        <v>1000</v>
       </c>
       <c r="E296" s="2"/>
       <c r="F296" s="2">
@@ -20757,7 +20764,7 @@
       </c>
       <c r="C297" s="15"/>
       <c r="D297" s="2" t="s">
-        <v>1089</v>
+        <v>1000</v>
       </c>
       <c r="E297" s="2"/>
       <c r="F297" s="2">
@@ -21507,10 +21514,10 @@
       </c>
       <c r="C314" s="15"/>
       <c r="D314" s="2" t="s">
-        <v>1090</v>
+        <v>1001</v>
       </c>
       <c r="E314" s="2" t="s">
-        <v>1091</v>
+        <v>1002</v>
       </c>
       <c r="F314" s="2">
         <v>2.96</v>
@@ -21555,10 +21562,10 @@
       </c>
       <c r="C315" s="15"/>
       <c r="D315" s="2" t="s">
-        <v>1090</v>
+        <v>1001</v>
       </c>
       <c r="E315" s="2" t="s">
-        <v>1092</v>
+        <v>1003</v>
       </c>
       <c r="F315" s="2">
         <v>3.14</v>
@@ -21643,7 +21650,7 @@
         <v>295</v>
       </c>
       <c r="B317" s="19" t="s">
-        <v>1147</v>
+        <v>1058</v>
       </c>
       <c r="C317" s="15"/>
       <c r="D317" s="2"/>
@@ -21687,7 +21694,7 @@
         <v>300</v>
       </c>
       <c r="B318" s="19" t="s">
-        <v>1148</v>
+        <v>1059</v>
       </c>
       <c r="C318" s="15"/>
       <c r="D318" s="2"/>
@@ -21731,7 +21738,7 @@
         <v>299</v>
       </c>
       <c r="B319" s="19" t="s">
-        <v>1149</v>
+        <v>1060</v>
       </c>
       <c r="C319" s="15"/>
       <c r="D319" s="2"/>
@@ -21775,7 +21782,7 @@
         <v>298</v>
       </c>
       <c r="B320" s="19" t="s">
-        <v>1150</v>
+        <v>1061</v>
       </c>
       <c r="C320" s="15"/>
       <c r="D320" s="2"/>
@@ -21819,7 +21826,7 @@
         <v>297</v>
       </c>
       <c r="B321" s="19" t="s">
-        <v>1151</v>
+        <v>1062</v>
       </c>
       <c r="C321" s="15"/>
       <c r="D321" s="2"/>
@@ -22178,7 +22185,7 @@
         <v>776</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>1152</v>
+        <v>1063</v>
       </c>
       <c r="F329" s="2">
         <v>2.17</v>
@@ -22358,7 +22365,7 @@
         <v>776</v>
       </c>
       <c r="E333" s="2" t="s">
-        <v>1094</v>
+        <v>1005</v>
       </c>
       <c r="F333" s="2">
         <v>3.03</v>
@@ -22396,17 +22403,17 @@
     </row>
     <row r="334" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A334" s="2" t="s">
-        <v>1093</v>
+        <v>1004</v>
       </c>
       <c r="B334" s="19" t="s">
-        <v>1153</v>
+        <v>1064</v>
       </c>
       <c r="C334" s="15"/>
       <c r="D334" s="2" t="s">
         <v>776</v>
       </c>
       <c r="E334" s="2" t="s">
-        <v>1095</v>
+        <v>1006</v>
       </c>
       <c r="F334" s="2">
         <v>2.1800000000000002</v>
@@ -22451,10 +22458,10 @@
       </c>
       <c r="C335" s="15"/>
       <c r="D335" s="2" t="s">
-        <v>1096</v>
+        <v>1007</v>
       </c>
       <c r="E335" s="2" t="s">
-        <v>1097</v>
+        <v>1008</v>
       </c>
       <c r="F335" s="2">
         <v>2.92</v>
@@ -22626,8 +22633,8 @@
       <c r="A339" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B339" s="15" t="s">
-        <v>926</v>
+      <c r="B339" s="20" t="s">
+        <v>1098</v>
       </c>
       <c r="C339" s="15"/>
       <c r="D339" s="2"/>
@@ -22670,8 +22677,8 @@
       <c r="A340" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B340" s="15" t="s">
-        <v>927</v>
+      <c r="B340" s="20" t="s">
+        <v>1099</v>
       </c>
       <c r="C340" s="15"/>
       <c r="D340" s="2"/>
@@ -22714,8 +22721,8 @@
       <c r="A341" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B341" s="15" t="s">
-        <v>928</v>
+      <c r="B341" s="20" t="s">
+        <v>1104</v>
       </c>
       <c r="C341" s="15"/>
       <c r="D341" s="2"/>
@@ -22758,8 +22765,8 @@
       <c r="A342" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B342" s="15" t="s">
-        <v>929</v>
+      <c r="B342" s="20" t="s">
+        <v>1103</v>
       </c>
       <c r="C342" s="15"/>
       <c r="D342" s="2"/>
@@ -22802,8 +22809,8 @@
       <c r="A343" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B343" s="15" t="s">
-        <v>930</v>
+      <c r="B343" s="20" t="s">
+        <v>1102</v>
       </c>
       <c r="C343" s="15"/>
       <c r="D343" s="2"/>
@@ -22846,8 +22853,8 @@
       <c r="A344" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B344" s="15" t="s">
-        <v>931</v>
+      <c r="B344" s="20" t="s">
+        <v>1101</v>
       </c>
       <c r="C344" s="15"/>
       <c r="D344" s="2"/>
@@ -22890,8 +22897,8 @@
       <c r="A345" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B345" s="15" t="s">
-        <v>932</v>
+      <c r="B345" s="20" t="s">
+        <v>1100</v>
       </c>
       <c r="C345" s="15"/>
       <c r="D345" s="2"/>
@@ -22934,8 +22941,8 @@
       <c r="A346" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B346" s="15" t="s">
-        <v>933</v>
+      <c r="B346" s="20" t="s">
+        <v>1097</v>
       </c>
       <c r="C346" s="15"/>
       <c r="D346" s="2"/>
@@ -22978,8 +22985,8 @@
       <c r="A347" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B347" s="15" t="s">
-        <v>934</v>
+      <c r="B347" s="20" t="s">
+        <v>1105</v>
       </c>
       <c r="C347" s="15"/>
       <c r="D347" s="2"/>
@@ -23022,8 +23029,8 @@
       <c r="A348" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B348" s="15" t="s">
-        <v>935</v>
+      <c r="B348" s="20" t="s">
+        <v>1106</v>
       </c>
       <c r="C348" s="15"/>
       <c r="D348" s="2"/>
@@ -23066,8 +23073,8 @@
       <c r="A349" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B349" s="15" t="s">
-        <v>936</v>
+      <c r="B349" s="20" t="s">
+        <v>1107</v>
       </c>
       <c r="C349" s="15"/>
       <c r="D349" s="2"/>
@@ -23110,8 +23117,8 @@
       <c r="A350" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B350" s="15" t="s">
-        <v>937</v>
+      <c r="B350" s="20" t="s">
+        <v>1108</v>
       </c>
       <c r="C350" s="15"/>
       <c r="D350" s="2"/>
@@ -23154,8 +23161,8 @@
       <c r="A351" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B351" s="15" t="s">
-        <v>932</v>
+      <c r="B351" s="20" t="s">
+        <v>1109</v>
       </c>
       <c r="C351" s="15"/>
       <c r="D351" s="2"/>
@@ -23199,7 +23206,7 @@
         <v>333</v>
       </c>
       <c r="B352" s="15" t="s">
-        <v>938</v>
+        <v>926</v>
       </c>
       <c r="C352" s="15"/>
       <c r="D352" s="2"/>
@@ -23243,7 +23250,7 @@
         <v>335</v>
       </c>
       <c r="B353" s="15" t="s">
-        <v>939</v>
+        <v>927</v>
       </c>
       <c r="C353" s="15"/>
       <c r="D353" s="2"/>
@@ -23331,7 +23338,7 @@
         <v>336</v>
       </c>
       <c r="B355" s="15" t="s">
-        <v>940</v>
+        <v>928</v>
       </c>
       <c r="C355" s="15"/>
       <c r="D355" s="2"/>
@@ -23375,7 +23382,7 @@
         <v>337</v>
       </c>
       <c r="B356" s="15" t="s">
-        <v>941</v>
+        <v>929</v>
       </c>
       <c r="C356" s="15"/>
       <c r="D356" s="2"/>
@@ -23419,7 +23426,7 @@
         <v>338</v>
       </c>
       <c r="B357" s="15" t="s">
-        <v>942</v>
+        <v>930</v>
       </c>
       <c r="C357" s="15"/>
       <c r="D357" s="2"/>
@@ -23535,7 +23542,7 @@
       </c>
       <c r="C360" s="17"/>
       <c r="D360" s="1" t="s">
-        <v>1154</v>
+        <v>1065</v>
       </c>
       <c r="F360" s="1">
         <v>2.4700000000000002</v>
@@ -23642,10 +23649,10 @@
     </row>
     <row r="363" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A363" s="2" t="s">
-        <v>345</v>
+        <v>4</v>
       </c>
       <c r="B363" s="15" t="s">
-        <v>943</v>
+        <v>789</v>
       </c>
       <c r="C363" s="15"/>
       <c r="D363" s="2"/>
@@ -23686,10 +23693,10 @@
     </row>
     <row r="364" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A364" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B364" s="15" t="s">
-        <v>944</v>
+        <v>1112</v>
+      </c>
+      <c r="B364" s="20" t="s">
+        <v>793</v>
       </c>
       <c r="C364" s="15"/>
       <c r="D364" s="2"/>
@@ -23730,10 +23737,10 @@
     </row>
     <row r="365" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A365" s="2" t="s">
-        <v>1155</v>
-      </c>
-      <c r="B365" s="19" t="s">
-        <v>1157</v>
+        <v>1113</v>
+      </c>
+      <c r="B365" s="20" t="s">
+        <v>1110</v>
       </c>
       <c r="C365" s="15"/>
       <c r="D365" s="2"/>
@@ -23774,10 +23781,10 @@
     </row>
     <row r="366" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A366" s="2" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B366" s="19" t="s">
-        <v>1158</v>
+        <v>1114</v>
+      </c>
+      <c r="B366" s="20" t="s">
+        <v>1111</v>
       </c>
       <c r="C366" s="15"/>
       <c r="D366" s="2"/>
@@ -23821,7 +23828,7 @@
         <v>349</v>
       </c>
       <c r="B367" s="15" t="s">
-        <v>945</v>
+        <v>931</v>
       </c>
       <c r="C367" s="15"/>
       <c r="D367" s="2"/>
@@ -23909,7 +23916,7 @@
         <v>352</v>
       </c>
       <c r="B369" s="19" t="s">
-        <v>1159</v>
+        <v>1066</v>
       </c>
       <c r="C369" s="15"/>
       <c r="D369" s="2"/>
@@ -23953,7 +23960,7 @@
         <v>353</v>
       </c>
       <c r="B370" s="15" t="s">
-        <v>946</v>
+        <v>932</v>
       </c>
       <c r="C370" s="15"/>
       <c r="D370" s="2"/>
@@ -23997,7 +24004,7 @@
         <v>354</v>
       </c>
       <c r="B371" s="19" t="s">
-        <v>1160</v>
+        <v>1067</v>
       </c>
       <c r="C371" s="15"/>
       <c r="D371" s="2"/>
@@ -24085,7 +24092,7 @@
         <v>355</v>
       </c>
       <c r="B373" s="19" t="s">
-        <v>1161</v>
+        <v>1068</v>
       </c>
       <c r="C373" s="15"/>
       <c r="D373" s="2"/>
@@ -24173,7 +24180,7 @@
         <v>357</v>
       </c>
       <c r="B375" s="19" t="s">
-        <v>1162</v>
+        <v>1069</v>
       </c>
       <c r="C375" s="15"/>
       <c r="D375" s="2"/>
@@ -24261,7 +24268,7 @@
         <v>359</v>
       </c>
       <c r="B377" s="15" t="s">
-        <v>947</v>
+        <v>933</v>
       </c>
       <c r="C377" s="15"/>
       <c r="D377" s="2"/>
@@ -24393,7 +24400,7 @@
         <v>360</v>
       </c>
       <c r="B380" s="15" t="s">
-        <v>948</v>
+        <v>934</v>
       </c>
       <c r="C380" s="15"/>
       <c r="D380" s="2"/>
@@ -24437,7 +24444,7 @@
         <v>355</v>
       </c>
       <c r="B381" s="19" t="s">
-        <v>1161</v>
+        <v>1068</v>
       </c>
       <c r="C381" s="15"/>
       <c r="D381" s="2"/>
@@ -24481,7 +24488,7 @@
         <v>357</v>
       </c>
       <c r="B382" s="19" t="s">
-        <v>1162</v>
+        <v>1069</v>
       </c>
       <c r="C382" s="15"/>
       <c r="D382" s="2"/>
@@ -24566,7 +24573,7 @@
     </row>
     <row r="384" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A384" s="2" t="s">
-        <v>1098</v>
+        <v>1009</v>
       </c>
       <c r="B384" s="15" t="s">
         <v>822</v>
@@ -24615,7 +24622,7 @@
         <v>365</v>
       </c>
       <c r="B385" s="15" t="s">
-        <v>949</v>
+        <v>935</v>
       </c>
       <c r="C385" s="15"/>
       <c r="D385" s="2"/>
@@ -24749,7 +24756,7 @@
         <v>369</v>
       </c>
       <c r="B388" s="15" t="s">
-        <v>950</v>
+        <v>936</v>
       </c>
       <c r="C388" s="15"/>
       <c r="D388" s="2"/>
@@ -24927,7 +24934,7 @@
         <v>375</v>
       </c>
       <c r="B392" s="19" t="s">
-        <v>1163</v>
+        <v>1070</v>
       </c>
       <c r="C392" s="15"/>
       <c r="D392" s="2"/>
@@ -24971,7 +24978,7 @@
         <v>377</v>
       </c>
       <c r="B393" s="15" t="s">
-        <v>951</v>
+        <v>937</v>
       </c>
       <c r="C393" s="15"/>
       <c r="D393" s="2"/>
@@ -25014,8 +25021,8 @@
       <c r="A394" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B394" s="15" t="s">
-        <v>952</v>
+      <c r="B394" s="20" t="s">
+        <v>1115</v>
       </c>
       <c r="C394" s="15"/>
       <c r="D394" s="2"/>
@@ -25058,8 +25065,8 @@
       <c r="A395" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B395" s="15" t="s">
-        <v>953</v>
+      <c r="B395" s="20" t="s">
+        <v>1116</v>
       </c>
       <c r="C395" s="15"/>
       <c r="D395" s="2"/>
@@ -25102,8 +25109,8 @@
       <c r="A396" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B396" s="15" t="s">
-        <v>954</v>
+      <c r="B396" s="20" t="s">
+        <v>1117</v>
       </c>
       <c r="C396" s="15"/>
       <c r="D396" s="2"/>
@@ -25146,8 +25153,8 @@
       <c r="A397" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B397" s="15" t="s">
-        <v>955</v>
+      <c r="B397" s="20" t="s">
+        <v>1118</v>
       </c>
       <c r="C397" s="15"/>
       <c r="D397" s="2"/>
@@ -25190,8 +25197,8 @@
       <c r="A398" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B398" s="15" t="s">
-        <v>956</v>
+      <c r="B398" s="20" t="s">
+        <v>1120</v>
       </c>
       <c r="C398" s="15"/>
       <c r="D398" s="2"/>
@@ -25234,8 +25241,8 @@
       <c r="A399" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B399" s="15" t="s">
-        <v>957</v>
+      <c r="B399" s="20" t="s">
+        <v>1119</v>
       </c>
       <c r="C399" s="15"/>
       <c r="D399" s="2"/>
@@ -25278,8 +25285,8 @@
       <c r="A400" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B400" s="15" t="s">
-        <v>958</v>
+      <c r="B400" s="20" t="s">
+        <v>1126</v>
       </c>
       <c r="C400" s="15"/>
       <c r="D400" s="2"/>
@@ -25322,8 +25329,8 @@
       <c r="A401" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B401" s="15" t="s">
-        <v>959</v>
+      <c r="B401" s="20" t="s">
+        <v>1125</v>
       </c>
       <c r="C401" s="15"/>
       <c r="D401" s="2"/>
@@ -25366,8 +25373,8 @@
       <c r="A402" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B402" s="15" t="s">
-        <v>960</v>
+      <c r="B402" s="20" t="s">
+        <v>1124</v>
       </c>
       <c r="C402" s="15"/>
       <c r="D402" s="2"/>
@@ -25410,8 +25417,8 @@
       <c r="A403" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B403" s="15" t="s">
-        <v>961</v>
+      <c r="B403" s="20" t="s">
+        <v>1123</v>
       </c>
       <c r="C403" s="15"/>
       <c r="D403" s="2"/>
@@ -25454,8 +25461,8 @@
       <c r="A404" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B404" s="15" t="s">
-        <v>962</v>
+      <c r="B404" s="20" t="s">
+        <v>1122</v>
       </c>
       <c r="C404" s="15"/>
       <c r="D404" s="2"/>
@@ -25498,8 +25505,8 @@
       <c r="A405" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B405" s="15" t="s">
-        <v>963</v>
+      <c r="B405" s="20" t="s">
+        <v>1121</v>
       </c>
       <c r="C405" s="15"/>
       <c r="D405" s="2"/>
@@ -25542,8 +25549,8 @@
       <c r="A406" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B406" s="15" t="s">
-        <v>964</v>
+      <c r="B406" s="20" t="s">
+        <v>938</v>
       </c>
       <c r="C406" s="15"/>
       <c r="D406" s="2"/>
@@ -25586,8 +25593,8 @@
       <c r="A407" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B407" s="15" t="s">
-        <v>965</v>
+      <c r="B407" s="20" t="s">
+        <v>1127</v>
       </c>
       <c r="C407" s="15"/>
       <c r="D407" s="2"/>
@@ -25630,8 +25637,8 @@
       <c r="A408" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B408" s="15" t="s">
-        <v>966</v>
+      <c r="B408" s="20" t="s">
+        <v>1128</v>
       </c>
       <c r="C408" s="15"/>
       <c r="D408" s="2"/>
@@ -25674,8 +25681,8 @@
       <c r="A409" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B409" s="15" t="s">
-        <v>967</v>
+      <c r="B409" s="20" t="s">
+        <v>1129</v>
       </c>
       <c r="C409" s="15"/>
       <c r="D409" s="2"/>
@@ -25718,8 +25725,8 @@
       <c r="A410" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B410" s="15" t="s">
-        <v>968</v>
+      <c r="B410" s="20" t="s">
+        <v>1130</v>
       </c>
       <c r="C410" s="15"/>
       <c r="D410" s="2"/>
@@ -25762,8 +25769,8 @@
       <c r="A411" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B411" s="15" t="s">
-        <v>969</v>
+      <c r="B411" s="20" t="s">
+        <v>1131</v>
       </c>
       <c r="C411" s="15"/>
       <c r="D411" s="2"/>
@@ -25806,8 +25813,8 @@
       <c r="A412" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B412" s="15" t="s">
-        <v>970</v>
+      <c r="B412" s="20" t="s">
+        <v>1132</v>
       </c>
       <c r="C412" s="15"/>
       <c r="D412" s="2"/>
@@ -25850,8 +25857,8 @@
       <c r="A413" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B413" s="15" t="s">
-        <v>971</v>
+      <c r="B413" s="20" t="s">
+        <v>1133</v>
       </c>
       <c r="C413" s="15"/>
       <c r="D413" s="2"/>
@@ -25894,8 +25901,8 @@
       <c r="A414" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B414" s="15" t="s">
-        <v>972</v>
+      <c r="B414" s="20" t="s">
+        <v>1134</v>
       </c>
       <c r="C414" s="15"/>
       <c r="D414" s="2"/>
@@ -25938,8 +25945,8 @@
       <c r="A415" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B415" s="15" t="s">
-        <v>973</v>
+      <c r="B415" s="20" t="s">
+        <v>1135</v>
       </c>
       <c r="C415" s="15"/>
       <c r="D415" s="2"/>
@@ -25982,8 +25989,8 @@
       <c r="A416" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B416" s="15" t="s">
-        <v>974</v>
+      <c r="B416" s="20" t="s">
+        <v>1136</v>
       </c>
       <c r="C416" s="15"/>
       <c r="D416" s="2"/>
@@ -26026,8 +26033,8 @@
       <c r="A417" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B417" s="15" t="s">
-        <v>975</v>
+      <c r="B417" s="20" t="s">
+        <v>1137</v>
       </c>
       <c r="C417" s="15"/>
       <c r="D417" s="2"/>
@@ -26070,8 +26077,8 @@
       <c r="A418" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B418" s="15" t="s">
-        <v>976</v>
+      <c r="B418" s="20" t="s">
+        <v>1138</v>
       </c>
       <c r="C418" s="15"/>
       <c r="D418" s="2"/>
@@ -26290,8 +26297,8 @@
       <c r="A423" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B423" s="15" t="s">
-        <v>977</v>
+      <c r="B423" s="20" t="s">
+        <v>1139</v>
       </c>
       <c r="C423" s="15"/>
       <c r="D423" s="2"/>
@@ -26334,8 +26341,8 @@
       <c r="A424" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B424" s="15" t="s">
-        <v>978</v>
+      <c r="B424" s="20" t="s">
+        <v>1140</v>
       </c>
       <c r="C424" s="15"/>
       <c r="D424" s="2"/>
@@ -26378,8 +26385,8 @@
       <c r="A425" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B425" s="15" t="s">
-        <v>979</v>
+      <c r="B425" s="20" t="s">
+        <v>1141</v>
       </c>
       <c r="C425" s="15"/>
       <c r="D425" s="2"/>
@@ -26422,8 +26429,8 @@
       <c r="A426" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B426" s="15" t="s">
-        <v>980</v>
+      <c r="B426" s="20" t="s">
+        <v>1142</v>
       </c>
       <c r="C426" s="15"/>
       <c r="D426" s="2"/>
@@ -26466,8 +26473,8 @@
       <c r="A427" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B427" s="15" t="s">
-        <v>981</v>
+      <c r="B427" s="20" t="s">
+        <v>1143</v>
       </c>
       <c r="C427" s="15"/>
       <c r="D427" s="2"/>
@@ -26510,8 +26517,8 @@
       <c r="A428" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B428" s="15" t="s">
-        <v>982</v>
+      <c r="B428" s="20" t="s">
+        <v>1144</v>
       </c>
       <c r="C428" s="15"/>
       <c r="D428" s="2"/>
@@ -26596,10 +26603,10 @@
     </row>
     <row r="430" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A430" s="2" t="s">
-        <v>1164</v>
+        <v>1071</v>
       </c>
       <c r="B430" s="19" t="s">
-        <v>1166</v>
+        <v>1073</v>
       </c>
       <c r="C430" s="15"/>
       <c r="D430" s="2"/>
@@ -26640,10 +26647,10 @@
     </row>
     <row r="431" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A431" s="2" t="s">
-        <v>1165</v>
+        <v>1072</v>
       </c>
       <c r="B431" s="19" t="s">
-        <v>1167</v>
+        <v>1074</v>
       </c>
       <c r="C431" s="15"/>
       <c r="D431" s="2"/>
@@ -26687,7 +26694,7 @@
         <v>414</v>
       </c>
       <c r="B432" s="15" t="s">
-        <v>983</v>
+        <v>939</v>
       </c>
       <c r="C432" s="15"/>
       <c r="D432" s="2"/>
@@ -26775,7 +26782,7 @@
         <v>416</v>
       </c>
       <c r="B434" s="15" t="s">
-        <v>984</v>
+        <v>940</v>
       </c>
       <c r="C434" s="15"/>
       <c r="D434" s="2"/>
@@ -26863,7 +26870,7 @@
         <v>417</v>
       </c>
       <c r="B436" s="15" t="s">
-        <v>985</v>
+        <v>941</v>
       </c>
       <c r="C436" s="15"/>
       <c r="D436" s="2"/>
@@ -27036,10 +27043,10 @@
     </row>
     <row r="440" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A440" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="B440" s="15" t="s">
-        <v>986</v>
+        <v>429</v>
+      </c>
+      <c r="B440" s="20" t="s">
+        <v>1145</v>
       </c>
       <c r="C440" s="15"/>
       <c r="D440" s="2"/>
@@ -27080,10 +27087,10 @@
     </row>
     <row r="441" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A441" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="B441" s="15" t="s">
-        <v>987</v>
+        <v>406</v>
+      </c>
+      <c r="B441" s="20" t="s">
+        <v>1146</v>
       </c>
       <c r="C441" s="15"/>
       <c r="D441" s="2"/>
@@ -27127,7 +27134,7 @@
         <v>419</v>
       </c>
       <c r="B442" s="15" t="s">
-        <v>988</v>
+        <v>942</v>
       </c>
       <c r="C442" s="15"/>
       <c r="D442" s="2"/>
@@ -27170,8 +27177,8 @@
       <c r="A443" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B443" s="15" t="s">
-        <v>989</v>
+      <c r="B443" s="20" t="s">
+        <v>1147</v>
       </c>
       <c r="C443" s="15"/>
       <c r="D443" s="2"/>
@@ -27214,8 +27221,8 @@
       <c r="A444" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B444" s="15" t="s">
-        <v>990</v>
+      <c r="B444" s="20" t="s">
+        <v>1148</v>
       </c>
       <c r="C444" s="15"/>
       <c r="D444" s="2"/>
@@ -27302,8 +27309,8 @@
       <c r="A446" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B446" s="15" t="s">
-        <v>991</v>
+      <c r="B446" s="20" t="s">
+        <v>1149</v>
       </c>
       <c r="C446" s="15"/>
       <c r="D446" s="2"/>
@@ -27346,8 +27353,8 @@
       <c r="A447" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B447" s="19" t="s">
-        <v>992</v>
+      <c r="B447" s="20" t="s">
+        <v>1150</v>
       </c>
       <c r="C447" s="15"/>
       <c r="D447" s="2"/>
@@ -27390,8 +27397,8 @@
       <c r="A448" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B448" s="19" t="s">
-        <v>993</v>
+      <c r="B448" s="20" t="s">
+        <v>1151</v>
       </c>
       <c r="C448" s="15"/>
       <c r="D448" s="2"/>
@@ -27434,8 +27441,8 @@
       <c r="A449" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B449" s="15" t="s">
-        <v>994</v>
+      <c r="B449" s="20" t="s">
+        <v>1152</v>
       </c>
       <c r="C449" s="15"/>
       <c r="D449" s="2"/>
@@ -27478,8 +27485,8 @@
       <c r="A450" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B450" s="15" t="s">
-        <v>995</v>
+      <c r="B450" s="20" t="s">
+        <v>1153</v>
       </c>
       <c r="C450" s="15"/>
       <c r="D450" s="2"/>
@@ -27522,8 +27529,8 @@
       <c r="A451" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B451" s="15" t="s">
-        <v>996</v>
+      <c r="B451" s="20" t="s">
+        <v>1154</v>
       </c>
       <c r="C451" s="15"/>
       <c r="D451" s="2"/>
@@ -27567,7 +27574,7 @@
         <v>414</v>
       </c>
       <c r="B452" s="15" t="s">
-        <v>983</v>
+        <v>939</v>
       </c>
       <c r="C452" s="15"/>
       <c r="D452" s="2"/>
@@ -27610,8 +27617,8 @@
       <c r="A453" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B453" s="15" t="s">
-        <v>997</v>
+      <c r="B453" s="20" t="s">
+        <v>1155</v>
       </c>
       <c r="C453" s="15"/>
       <c r="D453" s="2"/>
@@ -27654,8 +27661,8 @@
       <c r="A454" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="B454" s="15" t="s">
-        <v>998</v>
+      <c r="B454" s="20" t="s">
+        <v>1147</v>
       </c>
       <c r="C454" s="15"/>
       <c r="D454" s="2"/>
@@ -27698,8 +27705,8 @@
       <c r="A455" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B455" s="15" t="s">
-        <v>999</v>
+      <c r="B455" s="20" t="s">
+        <v>1156</v>
       </c>
       <c r="C455" s="15"/>
       <c r="D455" s="2"/>
@@ -27742,8 +27749,8 @@
       <c r="A456" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B456" s="15" t="s">
-        <v>1000</v>
+      <c r="B456" s="20" t="s">
+        <v>1157</v>
       </c>
       <c r="C456" s="15"/>
       <c r="D456" s="2"/>
@@ -27786,8 +27793,8 @@
       <c r="A457" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B457" s="15" t="s">
-        <v>1001</v>
+      <c r="B457" s="20" t="s">
+        <v>1158</v>
       </c>
       <c r="C457" s="15"/>
       <c r="D457" s="2"/>
@@ -27830,8 +27837,8 @@
       <c r="A458" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B458" s="15" t="s">
-        <v>1002</v>
+      <c r="B458" s="20" t="s">
+        <v>1159</v>
       </c>
       <c r="C458" s="15"/>
       <c r="D458" s="2"/>
@@ -27874,8 +27881,8 @@
       <c r="A459" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B459" s="15" t="s">
-        <v>1003</v>
+      <c r="B459" s="20" t="s">
+        <v>1160</v>
       </c>
       <c r="C459" s="15"/>
       <c r="D459" s="2"/>
@@ -27918,8 +27925,8 @@
       <c r="A460" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="B460" s="15" t="s">
-        <v>1004</v>
+      <c r="B460" s="20" t="s">
+        <v>1148</v>
       </c>
       <c r="C460" s="15"/>
       <c r="D460" s="2"/>
@@ -27962,8 +27969,8 @@
       <c r="A461" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="B461" s="15" t="s">
-        <v>1005</v>
+      <c r="B461" s="20" t="s">
+        <v>1161</v>
       </c>
       <c r="C461" s="15"/>
       <c r="D461" s="2"/>
@@ -28006,8 +28013,8 @@
       <c r="A462" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B462" s="15" t="s">
-        <v>1006</v>
+      <c r="B462" s="20" t="s">
+        <v>1162</v>
       </c>
       <c r="C462" s="15"/>
       <c r="D462" s="2"/>
@@ -28050,8 +28057,8 @@
       <c r="A463" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B463" s="15" t="s">
-        <v>1007</v>
+      <c r="B463" s="20" t="s">
+        <v>1163</v>
       </c>
       <c r="C463" s="15"/>
       <c r="D463" s="2"/>
@@ -28094,8 +28101,8 @@
       <c r="A464" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="B464" s="15" t="s">
-        <v>1008</v>
+      <c r="B464" s="20" t="s">
+        <v>1164</v>
       </c>
       <c r="C464" s="15"/>
       <c r="D464" s="2"/>
@@ -28139,7 +28146,7 @@
         <v>445</v>
       </c>
       <c r="B465" s="15" t="s">
-        <v>1009</v>
+        <v>943</v>
       </c>
       <c r="C465" s="15"/>
       <c r="D465" s="2"/>
@@ -28182,8 +28189,8 @@
       <c r="A466" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B466" s="15" t="s">
-        <v>1010</v>
+      <c r="B466" s="20" t="s">
+        <v>1165</v>
       </c>
       <c r="C466" s="15"/>
       <c r="D466" s="2"/>
@@ -28226,8 +28233,8 @@
       <c r="A467" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B467" s="15" t="s">
-        <v>1011</v>
+      <c r="B467" s="20" t="s">
+        <v>1166</v>
       </c>
       <c r="C467" s="15"/>
       <c r="D467" s="2"/>
@@ -28270,8 +28277,8 @@
       <c r="A468" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="B468" s="15" t="s">
-        <v>1012</v>
+      <c r="B468" s="20" t="s">
+        <v>1167</v>
       </c>
       <c r="C468" s="15"/>
       <c r="D468" s="2"/>
@@ -28314,8 +28321,8 @@
       <c r="A469" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B469" s="15" t="s">
-        <v>1013</v>
+      <c r="B469" s="20" t="s">
+        <v>1168</v>
       </c>
       <c r="C469" s="15"/>
       <c r="D469" s="2"/>
@@ -28358,8 +28365,8 @@
       <c r="A470" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B470" s="15" t="s">
-        <v>1014</v>
+      <c r="B470" s="20" t="s">
+        <v>1169</v>
       </c>
       <c r="C470" s="15"/>
       <c r="D470" s="2"/>
@@ -28402,8 +28409,8 @@
       <c r="A471" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B471" s="15" t="s">
-        <v>1015</v>
+      <c r="B471" s="20" t="s">
+        <v>1170</v>
       </c>
       <c r="C471" s="15"/>
       <c r="D471" s="2"/>
@@ -28446,8 +28453,8 @@
       <c r="A472" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="15" t="s">
-        <v>1016</v>
+      <c r="B472" s="20" t="s">
+        <v>1171</v>
       </c>
       <c r="C472" s="15"/>
       <c r="D472" s="2"/>
@@ -28490,8 +28497,8 @@
       <c r="A473" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B473" s="15" t="s">
-        <v>1017</v>
+      <c r="B473" s="20" t="s">
+        <v>1172</v>
       </c>
       <c r="C473" s="15"/>
       <c r="D473" s="2"/>
@@ -28534,8 +28541,8 @@
       <c r="A474" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="B474" s="15" t="s">
-        <v>1018</v>
+      <c r="B474" s="20" t="s">
+        <v>1173</v>
       </c>
       <c r="C474" s="15"/>
       <c r="D474" s="2"/>
@@ -28578,8 +28585,8 @@
       <c r="A475" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="B475" s="15" t="s">
-        <v>1019</v>
+      <c r="B475" s="20" t="s">
+        <v>1174</v>
       </c>
       <c r="C475" s="15"/>
       <c r="D475" s="2"/>
@@ -28622,8 +28629,8 @@
       <c r="A476" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B476" s="15" t="s">
-        <v>1020</v>
+      <c r="B476" s="20" t="s">
+        <v>1175</v>
       </c>
       <c r="C476" s="15"/>
       <c r="D476" s="2"/>
@@ -28666,8 +28673,8 @@
       <c r="A477" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B477" s="15" t="s">
-        <v>1021</v>
+      <c r="B477" s="20" t="s">
+        <v>1176</v>
       </c>
       <c r="C477" s="15"/>
       <c r="D477" s="2"/>
@@ -28707,11 +28714,11 @@
       <c r="AD477" s="2"/>
     </row>
     <row r="478" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A478" s="2" t="s">
+      <c r="A478" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B478" s="15" t="s">
-        <v>1022</v>
+      <c r="B478" s="20" t="s">
+        <v>1177</v>
       </c>
       <c r="C478" s="15"/>
       <c r="D478" s="2"/>
@@ -28754,8 +28761,8 @@
       <c r="A479" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B479" s="15" t="s">
-        <v>1023</v>
+      <c r="B479" s="20" t="s">
+        <v>1178</v>
       </c>
       <c r="C479" s="15"/>
       <c r="D479" s="2"/>
@@ -28798,8 +28805,8 @@
       <c r="A480" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B480" s="15" t="s">
-        <v>1024</v>
+      <c r="B480" s="20" t="s">
+        <v>1179</v>
       </c>
       <c r="C480" s="15"/>
       <c r="D480" s="2"/>
@@ -28842,8 +28849,8 @@
       <c r="A481" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="B481" s="15" t="s">
-        <v>1025</v>
+      <c r="B481" s="20" t="s">
+        <v>1180</v>
       </c>
       <c r="C481" s="15"/>
       <c r="D481" s="2"/>
@@ -28886,8 +28893,8 @@
       <c r="A482" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B482" s="15" t="s">
-        <v>1026</v>
+      <c r="B482" s="20" t="s">
+        <v>1181</v>
       </c>
       <c r="C482" s="15"/>
       <c r="D482" s="2"/>
@@ -28930,8 +28937,8 @@
       <c r="A483" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B483" s="15" t="s">
-        <v>1027</v>
+      <c r="B483" s="20" t="s">
+        <v>1182</v>
       </c>
       <c r="C483" s="15"/>
       <c r="D483" s="2"/>
@@ -28974,8 +28981,8 @@
       <c r="A484" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B484" s="15" t="s">
-        <v>1028</v>
+      <c r="B484" s="20" t="s">
+        <v>1183</v>
       </c>
       <c r="C484" s="15"/>
       <c r="D484" s="2"/>
@@ -29019,7 +29026,7 @@
         <v>445</v>
       </c>
       <c r="B485" s="15" t="s">
-        <v>1009</v>
+        <v>943</v>
       </c>
       <c r="C485" s="15"/>
       <c r="D485" s="2"/>
@@ -29062,8 +29069,8 @@
       <c r="A486" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B486" s="15" t="s">
-        <v>1013</v>
+      <c r="B486" s="20" t="s">
+        <v>1184</v>
       </c>
       <c r="C486" s="15"/>
       <c r="D486" s="2"/>
@@ -29151,7 +29158,7 @@
         <v>468</v>
       </c>
       <c r="B488" s="19" t="s">
-        <v>1168</v>
+        <v>1075</v>
       </c>
       <c r="C488" s="15"/>
       <c r="D488" s="2"/>
@@ -29195,7 +29202,7 @@
         <v>469</v>
       </c>
       <c r="B489" s="19" t="s">
-        <v>1169</v>
+        <v>1076</v>
       </c>
       <c r="C489" s="15"/>
       <c r="D489" s="2"/>
@@ -29239,7 +29246,7 @@
         <v>470</v>
       </c>
       <c r="B490" s="19" t="s">
-        <v>1170</v>
+        <v>1077</v>
       </c>
       <c r="C490" s="15"/>
       <c r="D490" s="2"/>
@@ -29283,7 +29290,7 @@
         <v>471</v>
       </c>
       <c r="B491" s="19" t="s">
-        <v>1171</v>
+        <v>1078</v>
       </c>
       <c r="C491" s="15"/>
       <c r="D491" s="2"/>
@@ -29327,7 +29334,7 @@
         <v>472</v>
       </c>
       <c r="B492" s="19" t="s">
-        <v>1172</v>
+        <v>1079</v>
       </c>
       <c r="C492" s="15"/>
       <c r="D492" s="2"/>
@@ -29371,7 +29378,7 @@
         <v>473</v>
       </c>
       <c r="B493" s="19" t="s">
-        <v>1173</v>
+        <v>1080</v>
       </c>
       <c r="C493" s="15"/>
       <c r="D493" s="2"/>
@@ -29415,7 +29422,7 @@
         <v>474</v>
       </c>
       <c r="B494" s="19" t="s">
-        <v>1174</v>
+        <v>1081</v>
       </c>
       <c r="C494" s="15"/>
       <c r="D494" s="2"/>
@@ -29459,7 +29466,7 @@
         <v>476</v>
       </c>
       <c r="B495" s="19" t="s">
-        <v>1175</v>
+        <v>1082</v>
       </c>
       <c r="C495" s="15"/>
       <c r="D495" s="2"/>
@@ -29503,7 +29510,7 @@
         <v>106</v>
       </c>
       <c r="B496" s="19" t="s">
-        <v>1176</v>
+        <v>1083</v>
       </c>
       <c r="C496" s="15"/>
       <c r="D496" s="2"/>
@@ -29547,7 +29554,7 @@
         <v>478</v>
       </c>
       <c r="B497" s="15" t="s">
-        <v>1029</v>
+        <v>944</v>
       </c>
       <c r="C497" s="15"/>
       <c r="D497" s="2"/>
@@ -29635,7 +29642,7 @@
         <v>480</v>
       </c>
       <c r="B499" s="19" t="s">
-        <v>1177</v>
+        <v>1084</v>
       </c>
       <c r="C499" s="15"/>
       <c r="D499" s="2"/>
@@ -29771,7 +29778,7 @@
         <v>483</v>
       </c>
       <c r="B502" s="15" t="s">
-        <v>1030</v>
+        <v>945</v>
       </c>
       <c r="C502" s="15"/>
       <c r="D502" s="2"/>
@@ -29815,7 +29822,7 @@
         <v>484</v>
       </c>
       <c r="B503" s="15" t="s">
-        <v>1031</v>
+        <v>946</v>
       </c>
       <c r="C503" s="15"/>
       <c r="D503" s="2"/>
@@ -29859,7 +29866,7 @@
         <v>485</v>
       </c>
       <c r="B504" s="15" t="s">
-        <v>1032</v>
+        <v>947</v>
       </c>
       <c r="C504" s="15"/>
       <c r="D504" s="2"/>
@@ -29903,7 +29910,7 @@
         <v>486</v>
       </c>
       <c r="B505" s="15" t="s">
-        <v>1033</v>
+        <v>948</v>
       </c>
       <c r="C505" s="15"/>
       <c r="D505" s="2"/>
@@ -29947,7 +29954,7 @@
         <v>487</v>
       </c>
       <c r="B506" s="15" t="s">
-        <v>1034</v>
+        <v>949</v>
       </c>
       <c r="C506" s="15"/>
       <c r="D506" s="2"/>
@@ -29991,7 +29998,7 @@
         <v>488</v>
       </c>
       <c r="B507" s="15" t="s">
-        <v>1035</v>
+        <v>950</v>
       </c>
       <c r="C507" s="15"/>
       <c r="D507" s="2"/>
@@ -30035,7 +30042,7 @@
         <v>489</v>
       </c>
       <c r="B508" s="15" t="s">
-        <v>1036</v>
+        <v>951</v>
       </c>
       <c r="C508" s="15"/>
       <c r="D508" s="2"/>
@@ -30079,7 +30086,7 @@
         <v>496</v>
       </c>
       <c r="B509" s="15" t="s">
-        <v>1037</v>
+        <v>952</v>
       </c>
       <c r="C509" s="15"/>
       <c r="D509" s="2"/>
@@ -30123,7 +30130,7 @@
         <v>490</v>
       </c>
       <c r="B510" s="15" t="s">
-        <v>1038</v>
+        <v>953</v>
       </c>
       <c r="C510" s="15"/>
       <c r="D510" s="2"/>
@@ -30167,7 +30174,7 @@
         <v>491</v>
       </c>
       <c r="B511" s="15" t="s">
-        <v>1039</v>
+        <v>954</v>
       </c>
       <c r="C511" s="15"/>
       <c r="D511" s="2"/>
@@ -30211,7 +30218,7 @@
         <v>492</v>
       </c>
       <c r="B512" s="15" t="s">
-        <v>1040</v>
+        <v>955</v>
       </c>
       <c r="C512" s="15"/>
       <c r="D512" s="2"/>
@@ -30255,7 +30262,7 @@
         <v>493</v>
       </c>
       <c r="B513" s="15" t="s">
-        <v>1041</v>
+        <v>956</v>
       </c>
       <c r="C513" s="15"/>
       <c r="D513" s="2"/>
@@ -30299,7 +30306,7 @@
         <v>494</v>
       </c>
       <c r="B514" s="15" t="s">
-        <v>1042</v>
+        <v>957</v>
       </c>
       <c r="C514" s="15"/>
       <c r="D514" s="2"/>
@@ -30343,7 +30350,7 @@
         <v>495</v>
       </c>
       <c r="B515" s="15" t="s">
-        <v>1043</v>
+        <v>958</v>
       </c>
       <c r="C515" s="15"/>
       <c r="D515" s="2"/>
@@ -30435,7 +30442,7 @@
       </c>
       <c r="C517" s="15"/>
       <c r="D517" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E517" s="2">
         <v>1</v>
@@ -30478,8 +30485,8 @@
       <c r="A518" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B518" s="15" t="s">
-        <v>991</v>
+      <c r="B518" s="20" t="s">
+        <v>1185</v>
       </c>
       <c r="C518" s="15"/>
       <c r="D518" s="2"/>
@@ -30522,8 +30529,8 @@
       <c r="A519" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B519" s="15" t="s">
-        <v>994</v>
+      <c r="B519" s="20" t="s">
+        <v>1186</v>
       </c>
       <c r="C519" s="15"/>
       <c r="D519" s="2"/>
@@ -30566,8 +30573,8 @@
       <c r="A520" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B520" s="15" t="s">
-        <v>996</v>
+      <c r="B520" s="20" t="s">
+        <v>1187</v>
       </c>
       <c r="C520" s="15"/>
       <c r="D520" s="2"/>
@@ -30610,12 +30617,12 @@
       <c r="A521" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B521" s="15" t="s">
-        <v>1044</v>
+      <c r="B521" s="20" t="s">
+        <v>1185</v>
       </c>
       <c r="C521" s="15"/>
       <c r="D521" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E521" s="2">
         <v>1</v>
@@ -30658,12 +30665,12 @@
       <c r="A522" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="B522" s="15" t="s">
-        <v>1045</v>
+      <c r="B522" s="20" t="s">
+        <v>1186</v>
       </c>
       <c r="C522" s="15"/>
       <c r="D522" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E522" s="2">
         <v>1</v>
@@ -30706,12 +30713,12 @@
       <c r="A523" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="B523" s="15" t="s">
-        <v>1046</v>
+      <c r="B523" s="20" t="s">
+        <v>1187</v>
       </c>
       <c r="C523" s="15"/>
       <c r="D523" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E523" s="2">
         <v>1</v>
@@ -30754,12 +30761,12 @@
       <c r="A524" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="B524" s="15" t="s">
-        <v>1044</v>
+      <c r="B524" s="20" t="s">
+        <v>1185</v>
       </c>
       <c r="C524" s="15"/>
       <c r="D524" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E524" s="2">
         <v>1</v>
@@ -30802,12 +30809,12 @@
       <c r="A525" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B525" s="15" t="s">
-        <v>1045</v>
+      <c r="B525" s="20" t="s">
+        <v>1186</v>
       </c>
       <c r="C525" s="15"/>
       <c r="D525" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E525" s="2">
         <v>1</v>
@@ -30850,12 +30857,12 @@
       <c r="A526" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="B526" s="15" t="s">
-        <v>1046</v>
+      <c r="B526" s="20" t="s">
+        <v>1187</v>
       </c>
       <c r="C526" s="15"/>
       <c r="D526" s="2" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="E526" s="2">
         <v>1</v>
@@ -52531,7 +52538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -52544,10 +52551,10 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>1179</v>
+        <v>1086</v>
       </c>
       <c r="C1" t="s">
-        <v>1180</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
@@ -52558,7 +52565,7 @@
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>1183</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
@@ -52569,7 +52576,7 @@
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>1184</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
@@ -52582,7 +52589,7 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>1090</v>
+        <v>1001</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -52590,13 +52597,13 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>1178</v>
+        <v>1085</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="P6" t="s">
-        <v>1185</v>
+        <v>1092</v>
       </c>
       <c r="Q6">
         <v>194</v>
@@ -52610,7 +52617,7 @@
         <v>17</v>
       </c>
       <c r="P7" t="s">
-        <v>1186</v>
+        <v>1093</v>
       </c>
       <c r="Q7">
         <v>148</v>
@@ -52618,7 +52625,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>1056</v>
+        <v>968</v>
       </c>
       <c r="C8">
         <v>21</v>
@@ -52626,7 +52633,7 @@
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>1096</v>
+        <v>1007</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -52634,7 +52641,7 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>1181</v>
+        <v>1088</v>
       </c>
       <c r="C10">
         <f>SUM(C2:C9)</f>
@@ -52643,7 +52650,7 @@
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>1182</v>
+        <v>1089</v>
       </c>
       <c r="C11">
         <f>525-52</f>
@@ -52660,7 +52667,7 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>1187</v>
+        <v>1094</v>
       </c>
       <c r="C14">
         <f>525-C13</f>

</xml_diff>